<commit_message>
conditional parallel run added
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\qa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B533488-8618-4D93-B8A9-788C9EB94E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53D8D85-9A3E-48B8-9135-8AAB420DE7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>parallel_run</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45A51-54AD-4EB2-9CAD-EE9C14BB949C}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,9 +457,10 @@
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -463,8 +470,11 @@
       <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -473,6 +483,9 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
api test system added
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53D8D85-9A3E-48B8-9135-8AAB420DE7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF10709D-44E4-407E-B4BA-0C1031FC0224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>email</t>
   </si>
@@ -67,7 +67,13 @@
     <t>parallel_run</t>
   </si>
   <si>
-    <t>yes</t>
+    <t>test_item</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>api_url</t>
   </si>
 </sst>
 </file>
@@ -446,51 +452,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45A51-54AD-4EB2-9CAD-EE9C14BB949C}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{74098323-5AA0-4A17-BE1B-A4BE860FD756}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{74098323-5AA0-4A17-BE1B-A4BE860FD756}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
api, ui separation fixed
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF10709D-44E4-407E-B4BA-0C1031FC0224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE73E13D-4D3A-4157-91FF-0AF16F51C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,10 +70,10 @@
     <t>test_item</t>
   </si>
   <si>
+    <t>api_url</t>
+  </si>
+  <si>
     <t>api</t>
-  </si>
-  <si>
-    <t>api_url</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +470,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -505,7 +505,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
report send feature both both run
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE73E13D-4D3A-4157-91FF-0AF16F51C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5FD699-031A-4180-A291-4CB410AE3CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>email</t>
   </si>
@@ -73,7 +73,16 @@
     <t>api_url</t>
   </si>
   <si>
-    <t>api</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Meta-Race</t>
+  </si>
+  <si>
+    <t>Both</t>
   </si>
 </sst>
 </file>
@@ -452,65 +461,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B45A51-54AD-4EB2-9CAD-EE9C14BB949C}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{B779C158-0AC3-4D4D-8F6D-082936161A0C}">
+      <formula1>"UI, API, Both"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2 E2" xr:uid="{6D7E548D-DF6C-41D1-9D7D-2CC3F10FE47C}">
+      <formula1>"no, yes"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{600F529F-389B-40DA-A954-2414E55316AC}">
+      <formula1>"Chrome, Firefox, Edge, Opera"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{74098323-5AA0-4A17-BE1B-A4BE860FD756}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{74098323-5AA0-4A17-BE1B-A4BE860FD756}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
ui, api both report sending implemented
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597FF151-46B0-40E8-8455-1BBC322FD6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8894B20-BA5B-4D01-896B-A5C42E453850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
     <t>Meta-Race</t>
   </si>
   <si>
-    <t>Both</t>
+    <t>UI</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
config.json moved to project root
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8894B20-BA5B-4D01-896B-A5C42E453850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660807DF-2094-4CD3-A0A3-CD3B66EB1457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
project name added to send_mail
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660807DF-2094-4CD3-A0A3-CD3B66EB1457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA43886A-3808-4AD4-9076-4DB39B14628A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
     <t>Meta-Race</t>
   </si>
   <si>
-    <t>UI</t>
+    <t>Both</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
meta race automation started
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -1,63 +1,127 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFAD71B-924C-4FE6-B7A7-574E395D86D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="configuration" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="login" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="configuration" sheetId="1" r:id="rId1"/>
+    <sheet name="login" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>api_url</t>
+  </si>
+  <si>
+    <t>frontend_url</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>headless</t>
+  </si>
+  <si>
+    <t>parallel_run</t>
+  </si>
+  <si>
+    <t>test_item</t>
+  </si>
+  <si>
+    <t>Meta-Race</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>login_data</t>
+  </si>
+  <si>
+    <t>unidevgo.qa1@gmail.com</t>
+  </si>
+  <si>
+    <t>5946644Ss@</t>
+  </si>
+  <si>
+    <t>signup</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>https://new-qa.metadog.racing</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -90,98 +154,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -447,208 +453,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="15.5703125" customWidth="1" style="5" min="1" max="1"/>
-    <col width="17.7109375" customWidth="1" style="5" min="2" max="2"/>
-    <col width="45.7109375" customWidth="1" style="5" min="3" max="3"/>
-    <col width="15.85546875" customWidth="1" style="5" min="4" max="4"/>
-    <col width="12.85546875" customWidth="1" style="5" min="5" max="5"/>
-    <col width="17.140625" customWidth="1" style="5" min="6" max="6"/>
-    <col width="25.42578125" customWidth="1" style="5" min="7" max="7"/>
+    <col min="1" max="1" width="15.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="5">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Project</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>api_url</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>frontend_url</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>browser</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>headless</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>parallel_run</t>
-        </is>
-      </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>test_item</t>
-        </is>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" ht="30" customHeight="1" s="5">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>Meta-Race</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>https://new-qa.knights.app</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Chrome</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="inlineStr">
-        <is>
-          <t>Both</t>
-        </is>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation sqref="G2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"UI, API, Both"</formula1>
     </dataValidation>
-    <dataValidation sqref="F2 E2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2 E2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"no, yes"</formula1>
     </dataValidation>
-    <dataValidation sqref="D2" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Chrome, Firefox, Edge, Opera"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="18.140625" customWidth="1" style="5" min="1" max="1"/>
-    <col width="33.140625" customWidth="1" style="5" min="2" max="2"/>
-    <col width="17" customWidth="1" style="5" min="3" max="3"/>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="17" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" s="5"/>
-    <row r="2" ht="30" customHeight="1" s="5">
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>password</t>
-        </is>
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" ht="30" customHeight="1" s="5">
-      <c r="A3" s="6" t="inlineStr">
-        <is>
-          <t>login_data</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>unidevgo.qa1@gmail.com</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>5946644Ss@</t>
-        </is>
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8">
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>password</t>
-        </is>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>signup</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t>unidevgo.qa1@gmail.com</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="n">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1">
         <v>456789</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="C9" display="5946644Ss@" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C9" r:id="rId4" display="5946644Ss@" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
custom logger implemented with a class in utils
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7662E99-6610-4562-974E-3A79F705CB4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA8063D-C371-4EE1-98E5-1E9CCE86AF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
headless run fail fixed
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA8063D-C371-4EE1-98E5-1E9CCE86AF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DA8F39-FBCD-45AB-B292-5866041C65DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
-  <si>
-    <t>Project</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>api_url</t>
   </si>
@@ -71,10 +68,19 @@
     <t>signup</t>
   </si>
   <si>
-    <t>UI</t>
-  </si>
-  <si>
     <t>https://new-qa.metadog.racing</t>
+  </si>
+  <si>
+    <t>report_receiver</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>project_name</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,52 +475,59 @@
     <col min="5" max="5" width="12.85546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="17.140625" style="5" customWidth="1"/>
     <col min="7" max="7" width="25.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>16</v>
+      <c r="H2" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -522,7 +535,7 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"UI, API, Both"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2 E2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:F2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"no, yes"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0000-000002000000}">
@@ -552,37 +565,37 @@
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
         <v>456789</v>

</xml_diff>

<commit_message>
environment variables added for security
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DA8F39-FBCD-45AB-B292-5866041C65DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4989A38D-CDAB-4C87-A303-278DADBDBF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>api_url</t>
   </si>
@@ -74,13 +74,16 @@
     <t>report_receiver</t>
   </si>
   <si>
-    <t>Both</t>
-  </si>
-  <si>
     <t>project_name</t>
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>sompod123@gmail.com</t>
+  </si>
+  <si>
+    <t>API</t>
   </si>
 </sst>
 </file>
@@ -160,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -179,6 +182,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -463,7 +467,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +484,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -518,16 +522,16 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
homepage test writing complete
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4989A38D-CDAB-4C87-A303-278DADBDBF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025F03BC-6EE9-49CC-84B4-2AE9A48AABC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="2055" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <t>sompod123@gmail.com</t>
   </si>
   <si>
-    <t>API</t>
+    <t>UI</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
API data provider and flow changed to class based.
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71C6825-F94B-46EB-B0DE-74E1DF62C6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6BEFF2-E562-4D97-9AA3-D88970E1E592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="1575" windowWidth="24075" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,13 +80,13 @@
     <t>sompod123@gmail.com</t>
   </si>
   <si>
-    <t>https://api-qa.metadog.racing</t>
-  </si>
-  <si>
     <t>Chrome</t>
   </si>
   <si>
     <t>UI</t>
+  </si>
+  <si>
+    <t>https://api-dev.metadog.racing</t>
   </si>
 </sst>
 </file>
@@ -207,12 +207,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -497,7 +495,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +511,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -542,14 +540,14 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>19</v>
+      <c r="B2" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>17</v>
@@ -558,7 +556,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
api flow refactored to class based with log outputs and stored
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6BEFF2-E562-4D97-9AA3-D88970E1E592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61ACD36-16B6-43B5-825E-2D7980F99969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="1575" windowWidth="24075" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,10 +83,10 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>https://api-dev.metadog.racing</t>
+    <t>API</t>
+  </si>
+  <si>
+    <t>https://api-qa.metadog.racing</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
otp verification script updated
</commit_message>
<xml_diff>
--- a/test_data/qa_test_data.xlsx
+++ b/test_data/qa_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shampad\Desktop\projects\python_selenium_test_template\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61ACD36-16B6-43B5-825E-2D7980F99969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7097F170-AF82-48D7-89C1-72D05B4E3371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="1575" windowWidth="24075" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -210,7 +210,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,7 +494,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +539,7 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="7" t="s">

</xml_diff>